<commit_message>
Added a column to say whether code 3s were FPs or FNs
</commit_message>
<xml_diff>
--- a/data/detection_check/detection_checked.xlsx
+++ b/data/detection_check/detection_checked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumente\GitHub Desktop\nonsig-master-thesis\data\detection_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F20B2-6D2E-4335-B55B-8BF01CDF5280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79435EBF-023B-4483-8EA3-6D304977D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AD23AB57-CA30-4E58-9F2C-C1454FBBBFCD}"/>
+    <workbookView xWindow="-28920" yWindow="3015" windowWidth="29040" windowHeight="15720" xr2:uid="{AD23AB57-CA30-4E58-9F2C-C1454FBBBFCD}"/>
   </bookViews>
   <sheets>
     <sheet name="detection_checked" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="651">
   <si>
     <t>article_id</t>
   </si>
@@ -1911,9 +1911,6 @@
     <t>Papercheck says this statement is in the Intro, which is both wrong-ish and right-ish; there is no real header or section title, so even a human could really say it's the results, so code 1</t>
   </si>
   <si>
-    <t>No idea, where this sentence is coming from. I can't find it in the pdf. There are no p values in the text (just tables).</t>
-  </si>
-  <si>
     <t>Conversely, regarding generalization, there was no significant difference in SCR when participants viewed the CS+ than when they viewed the CS−, t(32) = 0.89, p = .382, d = 0.15.</t>
   </si>
   <si>
@@ -1972,6 +1969,32 @@
   </si>
   <si>
     <t>hallucination</t>
+  </si>
+  <si>
+    <t>agree_3_FP_FN</t>
+  </si>
+  <si>
+    <t>A keyword, summarizing why (possibly) the statement was not detected automatically</t>
+  </si>
+  <si>
+    <t>Comment on the 'agreement' classification</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>If 'agreement' was 3:
+FP = False Positive; the automatically detected statement was acutally not a statement with a nonsig. p value
+FN = False Negative; the automatically detected statement was incomplete or otherwise not usable due to an extraction error</t>
+  </si>
+  <si>
+    <t>No idea, where this sentence is coming from. I can't find it in the pdf. There are no p values in the text (only in tables).</t>
+  </si>
+  <si>
+    <t>Not sure why it did not get this one; possibly because of the ' '</t>
   </si>
 </sst>
 </file>
@@ -2921,10 +2944,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71956C31-B19E-4264-8709-1F2CE7C8CF56}">
-  <dimension ref="A1:Q193"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P168" sqref="P168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,10 +2959,10 @@
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="11" width="0" hidden="1" customWidth="1"/>
     <col min="12" max="14" width="50" style="5" customWidth="1"/>
-    <col min="15" max="17" width="12.85546875" style="5" customWidth="1"/>
+    <col min="15" max="18" width="12.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2985,13 +3009,16 @@
         <v>538</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>956797616647519</v>
       </c>
@@ -3039,8 +3066,9 @@
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="255" x14ac:dyDescent="0.25">
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>956797616647519</v>
       </c>
@@ -3088,8 +3116,9 @@
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>956797616665351</v>
       </c>
@@ -3137,8 +3166,9 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>956797616665351</v>
       </c>
@@ -3186,8 +3216,9 @@
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>956797616665351</v>
       </c>
@@ -3235,8 +3266,9 @@
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>956797617724435</v>
       </c>
@@ -3281,13 +3313,16 @@
         <v>3</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R7" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>956797616671327</v>
       </c>
@@ -3314,13 +3349,14 @@
         <v>2</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>956797616671327</v>
       </c>
@@ -3347,13 +3383,14 @@
         <v>2</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q9" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>956797616671327</v>
       </c>
@@ -3380,13 +3417,14 @@
         <v>2</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>956797616671327</v>
       </c>
@@ -3413,13 +3451,14 @@
         <v>2</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>956797616671327</v>
       </c>
@@ -3446,13 +3485,14 @@
         <v>2</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>956797616671327</v>
       </c>
@@ -3479,13 +3519,14 @@
         <v>2</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>956797616671327</v>
       </c>
@@ -3512,13 +3553,14 @@
         <v>2</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>956797616671327</v>
       </c>
@@ -3545,13 +3587,14 @@
         <v>2</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q15" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>956797618755322</v>
       </c>
@@ -3599,8 +3642,9 @@
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>956797618755322</v>
       </c>
@@ -3627,13 +3671,14 @@
         <v>2</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q17" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>956797618755322</v>
       </c>
@@ -3681,8 +3726,9 @@
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>956797618772822</v>
       </c>
@@ -3730,8 +3776,9 @@
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>956797618772822</v>
       </c>
@@ -3779,8 +3826,9 @@
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>956797618772822</v>
       </c>
@@ -3828,8 +3876,9 @@
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>956797618772822</v>
       </c>
@@ -3877,8 +3926,9 @@
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>956797618772822</v>
       </c>
@@ -3926,8 +3976,9 @@
       </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>956797618772822</v>
       </c>
@@ -3975,8 +4026,9 @@
       </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>956797618772822</v>
       </c>
@@ -4024,8 +4076,9 @@
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>956797618772822</v>
       </c>
@@ -4073,8 +4126,9 @@
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
-    </row>
-    <row r="27" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>956797618772822</v>
       </c>
@@ -4122,8 +4176,9 @@
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
-    </row>
-    <row r="28" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>956797618772822</v>
       </c>
@@ -4171,8 +4226,9 @@
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
-    </row>
-    <row r="29" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>956797618772822</v>
       </c>
@@ -4220,8 +4276,9 @@
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-    </row>
-    <row r="30" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>956797618772822</v>
       </c>
@@ -4269,8 +4326,9 @@
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R30" s="4"/>
+    </row>
+    <row r="31" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>956797618772822</v>
       </c>
@@ -4318,8 +4376,9 @@
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-    </row>
-    <row r="32" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>956797618772822</v>
       </c>
@@ -4367,8 +4426,9 @@
       </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-    </row>
-    <row r="33" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R32" s="4"/>
+    </row>
+    <row r="33" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>956797618772822</v>
       </c>
@@ -4416,8 +4476,9 @@
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-    </row>
-    <row r="34" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R33" s="4"/>
+    </row>
+    <row r="34" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>956797618772822</v>
       </c>
@@ -4465,8 +4526,9 @@
       </c>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-    </row>
-    <row r="35" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>956797618772822</v>
       </c>
@@ -4514,8 +4576,9 @@
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-    </row>
-    <row r="36" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>956797618772822</v>
       </c>
@@ -4563,8 +4626,9 @@
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-    </row>
-    <row r="37" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>956797618772822</v>
       </c>
@@ -4612,8 +4676,9 @@
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-    </row>
-    <row r="38" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R37" s="4"/>
+    </row>
+    <row r="38" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>956797618772822</v>
       </c>
@@ -4661,8 +4726,9 @@
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
-    </row>
-    <row r="39" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R38" s="4"/>
+    </row>
+    <row r="39" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>956797618772822</v>
       </c>
@@ -4710,8 +4776,9 @@
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
-    </row>
-    <row r="40" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R39" s="4"/>
+    </row>
+    <row r="40" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>956797618772822</v>
       </c>
@@ -4759,8 +4826,9 @@
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
-    </row>
-    <row r="41" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R40" s="4"/>
+    </row>
+    <row r="41" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>956797618772822</v>
       </c>
@@ -4807,13 +4875,16 @@
         <v>3</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="Q41" s="4" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R41" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>956797618772822</v>
       </c>
@@ -4861,8 +4932,9 @@
       </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
-    </row>
-    <row r="43" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R42" s="4"/>
+    </row>
+    <row r="43" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>956797618772822</v>
       </c>
@@ -4910,8 +4982,9 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
-    </row>
-    <row r="44" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R43" s="4"/>
+    </row>
+    <row r="44" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>956797618772822</v>
       </c>
@@ -4959,8 +5032,9 @@
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
-    </row>
-    <row r="45" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R44" s="4"/>
+    </row>
+    <row r="45" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>956797618772822</v>
       </c>
@@ -5008,8 +5082,9 @@
       </c>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
-    </row>
-    <row r="46" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R45" s="4"/>
+    </row>
+    <row r="46" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>956797619842261</v>
       </c>
@@ -5057,8 +5132,9 @@
       </c>
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
-    </row>
-    <row r="47" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R46" s="4"/>
+    </row>
+    <row r="47" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>956797619842261</v>
       </c>
@@ -5085,13 +5161,14 @@
         <v>2</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q47" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>956797619842261</v>
       </c>
@@ -5139,8 +5216,9 @@
       </c>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
-    </row>
-    <row r="49" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R48" s="4"/>
+    </row>
+    <row r="49" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>956797619842261</v>
       </c>
@@ -5188,8 +5266,9 @@
       </c>
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
-    </row>
-    <row r="50" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R49" s="4"/>
+    </row>
+    <row r="50" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>956797619842261</v>
       </c>
@@ -5216,13 +5295,14 @@
         <v>2</v>
       </c>
       <c r="P50" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q50" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R50" s="4"/>
+    </row>
+    <row r="51" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>956797619842261</v>
       </c>
@@ -5249,13 +5329,14 @@
         <v>2</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q51" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R51" s="4"/>
+    </row>
+    <row r="52" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>956797619842261</v>
       </c>
@@ -5282,13 +5363,14 @@
         <v>2</v>
       </c>
       <c r="P52" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q52" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R52" s="4"/>
+    </row>
+    <row r="53" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>956797619842261</v>
       </c>
@@ -5336,8 +5418,9 @@
       </c>
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
-    </row>
-    <row r="54" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R53" s="4"/>
+    </row>
+    <row r="54" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>956797619842261</v>
       </c>
@@ -5385,8 +5468,9 @@
       </c>
       <c r="P54" s="4"/>
       <c r="Q54" s="4"/>
-    </row>
-    <row r="55" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R54" s="4"/>
+    </row>
+    <row r="55" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>956797619842261</v>
       </c>
@@ -5413,13 +5497,14 @@
         <v>2</v>
       </c>
       <c r="P55" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q55" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R55" s="4"/>
+    </row>
+    <row r="56" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>956797619842261</v>
       </c>
@@ -5446,13 +5531,14 @@
         <v>2</v>
       </c>
       <c r="P56" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q56" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R56" s="4"/>
+    </row>
+    <row r="57" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>956797619842261</v>
       </c>
@@ -5479,13 +5565,14 @@
         <v>2</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q57" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R57" s="4"/>
+    </row>
+    <row r="58" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>956797619842261</v>
       </c>
@@ -5512,13 +5599,14 @@
         <v>2</v>
       </c>
       <c r="P58" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q58" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="R58" s="4"/>
+    </row>
+    <row r="59" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>956797619842261</v>
       </c>
@@ -5566,8 +5654,9 @@
       </c>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
-    </row>
-    <row r="60" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R59" s="4"/>
+    </row>
+    <row r="60" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>956797619842261</v>
       </c>
@@ -5594,13 +5683,14 @@
         <v>2</v>
       </c>
       <c r="P60" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q60" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R60" s="4"/>
+    </row>
+    <row r="61" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>956797619842261</v>
       </c>
@@ -5627,13 +5717,14 @@
         <v>2</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q61" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R61" s="4"/>
+    </row>
+    <row r="62" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>956797619842261</v>
       </c>
@@ -5681,8 +5772,9 @@
       </c>
       <c r="P62" s="4"/>
       <c r="Q62" s="4"/>
-    </row>
-    <row r="63" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R62" s="4"/>
+    </row>
+    <row r="63" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>956797619842261</v>
       </c>
@@ -5730,8 +5822,9 @@
       </c>
       <c r="P63" s="4"/>
       <c r="Q63" s="4"/>
-    </row>
-    <row r="64" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R63" s="4"/>
+    </row>
+    <row r="64" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>956797619842261</v>
       </c>
@@ -5779,8 +5872,9 @@
       </c>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
-    </row>
-    <row r="65" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R64" s="4"/>
+    </row>
+    <row r="65" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>956797619842261</v>
       </c>
@@ -5828,8 +5922,9 @@
       </c>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
-    </row>
-    <row r="66" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R65" s="4"/>
+    </row>
+    <row r="66" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>956797619842261</v>
       </c>
@@ -5856,13 +5951,14 @@
         <v>2</v>
       </c>
       <c r="P66" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q66" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R66" s="4"/>
+    </row>
+    <row r="67" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>956797619842261</v>
       </c>
@@ -5889,13 +5985,14 @@
         <v>2</v>
       </c>
       <c r="P67" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q67" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R67" s="4"/>
+    </row>
+    <row r="68" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>956797619842261</v>
       </c>
@@ -5943,8 +6040,9 @@
       </c>
       <c r="P68" s="4"/>
       <c r="Q68" s="4"/>
-    </row>
-    <row r="69" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R68" s="4"/>
+    </row>
+    <row r="69" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>956797619842261</v>
       </c>
@@ -5971,13 +6069,14 @@
         <v>2</v>
       </c>
       <c r="P69" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q69" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R69" s="4"/>
+    </row>
+    <row r="70" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>956797619842261</v>
       </c>
@@ -6025,8 +6124,9 @@
       </c>
       <c r="P70" s="4"/>
       <c r="Q70" s="4"/>
-    </row>
-    <row r="71" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+      <c r="R70" s="4"/>
+    </row>
+    <row r="71" spans="1:18" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>956797619842261</v>
       </c>
@@ -6074,8 +6174,9 @@
       </c>
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
-    </row>
-    <row r="72" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R71" s="4"/>
+    </row>
+    <row r="72" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>956797619842261</v>
       </c>
@@ -6102,13 +6203,14 @@
         <v>2</v>
       </c>
       <c r="P72" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q72" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="73" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R72" s="4"/>
+    </row>
+    <row r="73" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>956797619842261</v>
       </c>
@@ -6134,13 +6236,14 @@
         <v>2</v>
       </c>
       <c r="P73" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q73" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R73" s="4"/>
+    </row>
+    <row r="74" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>956797619869905</v>
       </c>
@@ -6188,8 +6291,9 @@
       </c>
       <c r="P74" s="4"/>
       <c r="Q74" s="4"/>
-    </row>
-    <row r="75" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R74" s="4"/>
+    </row>
+    <row r="75" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>956797619869905</v>
       </c>
@@ -6237,8 +6341,9 @@
       </c>
       <c r="P75" s="4"/>
       <c r="Q75" s="4"/>
-    </row>
-    <row r="76" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R75" s="4"/>
+    </row>
+    <row r="76" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>956797619869905</v>
       </c>
@@ -6286,8 +6391,9 @@
       </c>
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
-    </row>
-    <row r="77" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="R76" s="4"/>
+    </row>
+    <row r="77" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>956797619869905</v>
       </c>
@@ -6335,8 +6441,9 @@
       </c>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
-    </row>
-    <row r="78" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R77" s="4"/>
+    </row>
+    <row r="78" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>956797619869905</v>
       </c>
@@ -6384,8 +6491,9 @@
       </c>
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>
-    </row>
-    <row r="79" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R78" s="4"/>
+    </row>
+    <row r="79" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>956797619869905</v>
       </c>
@@ -6433,8 +6541,9 @@
       </c>
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
-    </row>
-    <row r="80" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R79" s="4"/>
+    </row>
+    <row r="80" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>956797619869905</v>
       </c>
@@ -6482,8 +6591,9 @@
       </c>
       <c r="P80" s="4"/>
       <c r="Q80" s="4"/>
-    </row>
-    <row r="81" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R80" s="4"/>
+    </row>
+    <row r="81" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>956797619869905</v>
       </c>
@@ -6531,8 +6641,9 @@
       </c>
       <c r="P81" s="4"/>
       <c r="Q81" s="4"/>
-    </row>
-    <row r="82" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="R81" s="4"/>
+    </row>
+    <row r="82" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>956797619869905</v>
       </c>
@@ -6580,8 +6691,9 @@
       </c>
       <c r="P82" s="4"/>
       <c r="Q82" s="4"/>
-    </row>
-    <row r="83" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R82" s="4"/>
+    </row>
+    <row r="83" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>956797619869905</v>
       </c>
@@ -6629,8 +6741,9 @@
       </c>
       <c r="P83" s="4"/>
       <c r="Q83" s="4"/>
-    </row>
-    <row r="84" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R83" s="4"/>
+    </row>
+    <row r="84" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>956797619890619</v>
       </c>
@@ -6658,8 +6771,9 @@
       <c r="Q84" s="4" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R84" s="4"/>
+    </row>
+    <row r="85" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>956797620951115</v>
       </c>
@@ -6687,8 +6801,9 @@
       <c r="Q85" s="4" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R85" s="4"/>
+    </row>
+    <row r="86" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>956797620965536</v>
       </c>
@@ -6738,8 +6853,9 @@
       <c r="Q86" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" ht="255" x14ac:dyDescent="0.25">
+      <c r="R86" s="4"/>
+    </row>
+    <row r="87" spans="1:18" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>956797620965536</v>
       </c>
@@ -6789,8 +6905,9 @@
       <c r="Q87" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R87" s="4"/>
+    </row>
+    <row r="88" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>956797620965536</v>
       </c>
@@ -6817,13 +6934,14 @@
         <v>2</v>
       </c>
       <c r="P88" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q88" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="89" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="R88" s="4"/>
+    </row>
+    <row r="89" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>956797620965536</v>
       </c>
@@ -6871,8 +6989,9 @@
       </c>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
-    </row>
-    <row r="90" spans="1:17" ht="360" x14ac:dyDescent="0.25">
+      <c r="R89" s="4"/>
+    </row>
+    <row r="90" spans="1:18" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>956797620965536</v>
       </c>
@@ -6920,8 +7039,9 @@
       </c>
       <c r="P90" s="4"/>
       <c r="Q90" s="4"/>
-    </row>
-    <row r="91" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="R90" s="4"/>
+    </row>
+    <row r="91" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>956797620965536</v>
       </c>
@@ -6969,8 +7089,9 @@
       </c>
       <c r="P91" s="4"/>
       <c r="Q91" s="4"/>
-    </row>
-    <row r="92" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R91" s="4"/>
+    </row>
+    <row r="92" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>956797620965536</v>
       </c>
@@ -7018,8 +7139,9 @@
       </c>
       <c r="P92" s="4"/>
       <c r="Q92" s="4"/>
-    </row>
-    <row r="93" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R92" s="4"/>
+    </row>
+    <row r="93" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>956797620965536</v>
       </c>
@@ -7067,8 +7189,9 @@
       </c>
       <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
-    </row>
-    <row r="94" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+      <c r="R93" s="4"/>
+    </row>
+    <row r="94" spans="1:18" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>956797620965536</v>
       </c>
@@ -7118,8 +7241,9 @@
       <c r="Q94" s="4" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="95" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R94" s="4"/>
+    </row>
+    <row r="95" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>956797620965536</v>
       </c>
@@ -7166,13 +7290,16 @@
         <v>3</v>
       </c>
       <c r="P95" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="Q95" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="Q95" s="4" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R95" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>956797620984464</v>
       </c>
@@ -7220,8 +7347,9 @@
       </c>
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
-    </row>
-    <row r="97" spans="1:17" ht="270" x14ac:dyDescent="0.25">
+      <c r="R96" s="4"/>
+    </row>
+    <row r="97" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>956797620984464</v>
       </c>
@@ -7269,8 +7397,9 @@
       </c>
       <c r="P97" s="4"/>
       <c r="Q97" s="4"/>
-    </row>
-    <row r="98" spans="1:17" ht="270" x14ac:dyDescent="0.25">
+      <c r="R97" s="4"/>
+    </row>
+    <row r="98" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>956797620984464</v>
       </c>
@@ -7318,8 +7447,9 @@
       </c>
       <c r="P98" s="4"/>
       <c r="Q98" s="4"/>
-    </row>
-    <row r="99" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="R98" s="4"/>
+    </row>
+    <row r="99" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>956797620984464</v>
       </c>
@@ -7367,8 +7497,9 @@
       </c>
       <c r="P99" s="4"/>
       <c r="Q99" s="4"/>
-    </row>
-    <row r="100" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R99" s="4"/>
+    </row>
+    <row r="100" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>956797620984464</v>
       </c>
@@ -7416,8 +7547,9 @@
       </c>
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
-    </row>
-    <row r="101" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R100" s="4"/>
+    </row>
+    <row r="101" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>956797620984464</v>
       </c>
@@ -7465,8 +7597,9 @@
       </c>
       <c r="P101" s="4"/>
       <c r="Q101" s="4"/>
-    </row>
-    <row r="102" spans="1:17" ht="390" x14ac:dyDescent="0.25">
+      <c r="R101" s="4"/>
+    </row>
+    <row r="102" spans="1:18" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>956797620984464</v>
       </c>
@@ -7514,8 +7647,9 @@
       </c>
       <c r="P102" s="4"/>
       <c r="Q102" s="4"/>
-    </row>
-    <row r="103" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="R102" s="4"/>
+    </row>
+    <row r="103" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>956797620984464</v>
       </c>
@@ -7563,8 +7697,9 @@
       </c>
       <c r="P103" s="4"/>
       <c r="Q103" s="4"/>
-    </row>
-    <row r="104" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R103" s="4"/>
+    </row>
+    <row r="104" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>956797620985832</v>
       </c>
@@ -7612,8 +7747,9 @@
       </c>
       <c r="P104" s="4"/>
       <c r="Q104" s="4"/>
-    </row>
-    <row r="105" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R104" s="4"/>
+    </row>
+    <row r="105" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>956797620985832</v>
       </c>
@@ -7661,8 +7797,9 @@
       </c>
       <c r="P105" s="4"/>
       <c r="Q105" s="4"/>
-    </row>
-    <row r="106" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R105" s="4"/>
+    </row>
+    <row r="106" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>956797620985832</v>
       </c>
@@ -7710,8 +7847,9 @@
       </c>
       <c r="P106" s="4"/>
       <c r="Q106" s="4"/>
-    </row>
-    <row r="107" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R106" s="4"/>
+    </row>
+    <row r="107" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>956797620985832</v>
       </c>
@@ -7759,8 +7897,9 @@
       </c>
       <c r="P107" s="4"/>
       <c r="Q107" s="4"/>
-    </row>
-    <row r="108" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R107" s="4"/>
+    </row>
+    <row r="108" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>956797620985832</v>
       </c>
@@ -7808,8 +7947,9 @@
       </c>
       <c r="P108" s="4"/>
       <c r="Q108" s="4"/>
-    </row>
-    <row r="109" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R108" s="4"/>
+    </row>
+    <row r="109" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>956797620985832</v>
       </c>
@@ -7857,8 +7997,9 @@
       </c>
       <c r="P109" s="4"/>
       <c r="Q109" s="4"/>
-    </row>
-    <row r="110" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R109" s="4"/>
+    </row>
+    <row r="110" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <v>956797620985832</v>
       </c>
@@ -7885,13 +8026,14 @@
         <v>2</v>
       </c>
       <c r="P110" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q110" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="111" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R110" s="4"/>
+    </row>
+    <row r="111" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <v>956797620985832</v>
       </c>
@@ -7939,8 +8081,9 @@
       </c>
       <c r="P111" s="4"/>
       <c r="Q111" s="4"/>
-    </row>
-    <row r="112" spans="1:17" ht="330" x14ac:dyDescent="0.25">
+      <c r="R111" s="4"/>
+    </row>
+    <row r="112" spans="1:18" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>956797620985832</v>
       </c>
@@ -7988,8 +8131,9 @@
       </c>
       <c r="P112" s="4"/>
       <c r="Q112" s="4"/>
-    </row>
-    <row r="113" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R112" s="4"/>
+    </row>
+    <row r="113" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>956797620985832</v>
       </c>
@@ -8037,8 +8181,9 @@
       </c>
       <c r="P113" s="4"/>
       <c r="Q113" s="4"/>
-    </row>
-    <row r="114" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R113" s="4"/>
+    </row>
+    <row r="114" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <v>956797621995197</v>
       </c>
@@ -8088,8 +8233,9 @@
       <c r="Q114" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="115" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R114" s="4"/>
+    </row>
+    <row r="115" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <v>956797621995197</v>
       </c>
@@ -8139,8 +8285,9 @@
       <c r="Q115" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="116" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R115" s="4"/>
+    </row>
+    <row r="116" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <v>956797621995197</v>
       </c>
@@ -8190,8 +8337,9 @@
       <c r="Q116" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="117" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R116" s="4"/>
+    </row>
+    <row r="117" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>956797621995197</v>
       </c>
@@ -8239,8 +8387,9 @@
       </c>
       <c r="P117" s="4"/>
       <c r="Q117" s="4"/>
-    </row>
-    <row r="118" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R117" s="4"/>
+    </row>
+    <row r="118" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>956797621995197</v>
       </c>
@@ -8288,8 +8437,9 @@
       </c>
       <c r="P118" s="4"/>
       <c r="Q118" s="4"/>
-    </row>
-    <row r="119" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R118" s="4"/>
+    </row>
+    <row r="119" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>956797621995197</v>
       </c>
@@ -8337,8 +8487,9 @@
       </c>
       <c r="P119" s="4"/>
       <c r="Q119" s="4"/>
-    </row>
-    <row r="120" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R119" s="4"/>
+    </row>
+    <row r="120" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>956797621995197</v>
       </c>
@@ -8386,8 +8537,9 @@
       </c>
       <c r="P120" s="4"/>
       <c r="Q120" s="4"/>
-    </row>
-    <row r="121" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R120" s="4"/>
+    </row>
+    <row r="121" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>956797621995197</v>
       </c>
@@ -8435,8 +8587,9 @@
       </c>
       <c r="P121" s="4"/>
       <c r="Q121" s="4"/>
-    </row>
-    <row r="122" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R121" s="4"/>
+    </row>
+    <row r="122" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <v>956797621995197</v>
       </c>
@@ -8463,13 +8616,14 @@
         <v>2</v>
       </c>
       <c r="P122" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q122" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="123" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R122" s="4"/>
+    </row>
+    <row r="123" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <v>956797621995197</v>
       </c>
@@ -8496,13 +8650,14 @@
         <v>2</v>
       </c>
       <c r="P123" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q123" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="124" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R123" s="4"/>
+    </row>
+    <row r="124" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <v>956797621995197</v>
       </c>
@@ -8550,8 +8705,9 @@
       </c>
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
-    </row>
-    <row r="125" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R124" s="4"/>
+    </row>
+    <row r="125" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>956797621995197</v>
       </c>
@@ -8599,8 +8755,9 @@
       </c>
       <c r="P125" s="4"/>
       <c r="Q125" s="4"/>
-    </row>
-    <row r="126" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R125" s="4"/>
+    </row>
+    <row r="126" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>956797621995197</v>
       </c>
@@ -8648,8 +8805,9 @@
       </c>
       <c r="P126" s="4"/>
       <c r="Q126" s="4"/>
-    </row>
-    <row r="127" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R126" s="4"/>
+    </row>
+    <row r="127" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>956797621995197</v>
       </c>
@@ -8697,8 +8855,9 @@
       </c>
       <c r="P127" s="4"/>
       <c r="Q127" s="4"/>
-    </row>
-    <row r="128" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R127" s="4"/>
+    </row>
+    <row r="128" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>956797621995197</v>
       </c>
@@ -8725,13 +8884,14 @@
         <v>2</v>
       </c>
       <c r="P128" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q128" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="129" spans="1:17" ht="300" x14ac:dyDescent="0.25">
+      <c r="R128" s="4"/>
+    </row>
+    <row r="129" spans="1:18" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>956797621995197</v>
       </c>
@@ -8779,8 +8939,9 @@
       </c>
       <c r="P129" s="4"/>
       <c r="Q129" s="4"/>
-    </row>
-    <row r="130" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R129" s="4"/>
+    </row>
+    <row r="130" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>956797621995197</v>
       </c>
@@ -8828,8 +8989,9 @@
       </c>
       <c r="P130" s="4"/>
       <c r="Q130" s="4"/>
-    </row>
-    <row r="131" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R130" s="4"/>
+    </row>
+    <row r="131" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <v>956797621995197</v>
       </c>
@@ -8856,13 +9018,14 @@
         <v>2</v>
       </c>
       <c r="P131" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q131" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="132" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R131" s="4"/>
+    </row>
+    <row r="132" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>956797621995197</v>
       </c>
@@ -8910,8 +9073,9 @@
       </c>
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
-    </row>
-    <row r="133" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R132" s="4"/>
+    </row>
+    <row r="133" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <v>956797621995197</v>
       </c>
@@ -8938,13 +9102,14 @@
         <v>2</v>
       </c>
       <c r="P133" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q133" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="134" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R133" s="4"/>
+    </row>
+    <row r="134" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>956797621995197</v>
       </c>
@@ -8992,8 +9157,9 @@
       </c>
       <c r="P134" s="4"/>
       <c r="Q134" s="4"/>
-    </row>
-    <row r="135" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R134" s="4"/>
+    </row>
+    <row r="135" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <v>956797621995197</v>
       </c>
@@ -9020,13 +9186,14 @@
         <v>2</v>
       </c>
       <c r="P135" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q135" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="136" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R135" s="4"/>
+    </row>
+    <row r="136" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <v>956797621995197</v>
       </c>
@@ -9073,13 +9240,16 @@
         <v>3</v>
       </c>
       <c r="P136" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="Q136" s="4" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="137" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R136" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <v>956797621995197</v>
       </c>
@@ -9127,8 +9297,9 @@
       </c>
       <c r="P137" s="4"/>
       <c r="Q137" s="4"/>
-    </row>
-    <row r="138" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R137" s="4"/>
+    </row>
+    <row r="138" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <v>956797621995197</v>
       </c>
@@ -9176,8 +9347,9 @@
       </c>
       <c r="P138" s="4"/>
       <c r="Q138" s="4"/>
-    </row>
-    <row r="139" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R138" s="4"/>
+    </row>
+    <row r="139" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <v>956797621995197</v>
       </c>
@@ -9204,13 +9376,14 @@
         <v>2</v>
       </c>
       <c r="P139" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q139" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="140" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R139" s="4"/>
+    </row>
+    <row r="140" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>956797621995197</v>
       </c>
@@ -9258,8 +9431,9 @@
       </c>
       <c r="P140" s="4"/>
       <c r="Q140" s="4"/>
-    </row>
-    <row r="141" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R140" s="4"/>
+    </row>
+    <row r="141" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>956797621995202</v>
       </c>
@@ -9307,8 +9481,9 @@
       </c>
       <c r="P141" s="4"/>
       <c r="Q141" s="4"/>
-    </row>
-    <row r="142" spans="1:17" ht="225" x14ac:dyDescent="0.25">
+      <c r="R141" s="4"/>
+    </row>
+    <row r="142" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>956797621995202</v>
       </c>
@@ -9356,8 +9531,9 @@
       </c>
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
-    </row>
-    <row r="143" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R142" s="4"/>
+    </row>
+    <row r="143" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <v>956797621995202</v>
       </c>
@@ -9384,13 +9560,14 @@
         <v>2</v>
       </c>
       <c r="P143" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q143" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="144" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R143" s="4"/>
+    </row>
+    <row r="144" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <v>956797621995202</v>
       </c>
@@ -9417,13 +9594,14 @@
         <v>2</v>
       </c>
       <c r="P144" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q144" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="145" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R144" s="4"/>
+    </row>
+    <row r="145" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>956797621995202</v>
       </c>
@@ -9471,8 +9649,9 @@
       </c>
       <c r="P145" s="4"/>
       <c r="Q145" s="4"/>
-    </row>
-    <row r="146" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R145" s="4"/>
+    </row>
+    <row r="146" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="9">
         <v>956797621995202</v>
       </c>
@@ -9499,13 +9678,14 @@
         <v>2</v>
       </c>
       <c r="P146" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q146" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="147" spans="1:17" ht="375" x14ac:dyDescent="0.25">
+      <c r="R146" s="4"/>
+    </row>
+    <row r="147" spans="1:18" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>956797621995202</v>
       </c>
@@ -9553,8 +9733,9 @@
       </c>
       <c r="P147" s="4"/>
       <c r="Q147" s="4"/>
-    </row>
-    <row r="148" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R147" s="4"/>
+    </row>
+    <row r="148" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <v>956797621995202</v>
       </c>
@@ -9581,13 +9762,14 @@
         <v>2</v>
       </c>
       <c r="P148" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q148" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="149" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R148" s="4"/>
+    </row>
+    <row r="149" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="9">
         <v>956797621995202</v>
       </c>
@@ -9614,13 +9796,14 @@
         <v>2</v>
       </c>
       <c r="P149" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q149" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="150" spans="1:17" ht="390" x14ac:dyDescent="0.25">
+      <c r="R149" s="4"/>
+    </row>
+    <row r="150" spans="1:18" ht="390" x14ac:dyDescent="0.25">
       <c r="A150" s="9">
         <v>9567976211005760</v>
       </c>
@@ -9667,13 +9850,16 @@
         <v>3</v>
       </c>
       <c r="P150" s="4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="Q150" s="4" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="151" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="R150" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <v>9567976211005760</v>
       </c>
@@ -9700,13 +9886,14 @@
         <v>2</v>
       </c>
       <c r="P151" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="Q151" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="152" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="R151" s="4"/>
+    </row>
+    <row r="152" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A152" s="9">
         <v>9567976211005760</v>
       </c>
@@ -9752,10 +9939,15 @@
       <c r="O152" s="4">
         <v>3</v>
       </c>
-      <c r="P152" s="4"/>
-      <c r="Q152" s="4"/>
-    </row>
-    <row r="153" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="P152" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q152" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="R152" s="4"/>
+    </row>
+    <row r="153" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <v>9567976211005760</v>
       </c>
@@ -9800,13 +9992,16 @@
         <v>3</v>
       </c>
       <c r="P153" s="4" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="Q153" s="4" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="154" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="R153" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <v>9567976211005760</v>
       </c>
@@ -9833,13 +10028,14 @@
         <v>2</v>
       </c>
       <c r="P154" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="Q154" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="155" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="R154" s="4"/>
+    </row>
+    <row r="155" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="9">
         <v>9567976211016390</v>
       </c>
@@ -9889,8 +10085,9 @@
       <c r="Q155" s="4" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="156" spans="1:17" ht="240" x14ac:dyDescent="0.25">
+      <c r="R155" s="4"/>
+    </row>
+    <row r="156" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <v>9567976211016390</v>
       </c>
@@ -9940,8 +10137,9 @@
       <c r="Q156" s="4" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="157" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R156" s="4"/>
+    </row>
+    <row r="157" spans="1:18" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <v>9567976211024260</v>
       </c>
@@ -9986,13 +10184,16 @@
         <v>3</v>
       </c>
       <c r="P157" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="Q157" s="4" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+      <c r="R157" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <v>9567976211028970</v>
       </c>
@@ -10042,8 +10243,9 @@
       <c r="Q158" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="159" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R158" s="4"/>
+    </row>
+    <row r="159" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <v>9567976211028970</v>
       </c>
@@ -10091,8 +10293,9 @@
       </c>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
-    </row>
-    <row r="160" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R159" s="4"/>
+    </row>
+    <row r="160" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="9">
         <v>9567976211028970</v>
       </c>
@@ -10140,8 +10343,9 @@
       </c>
       <c r="P160" s="4"/>
       <c r="Q160" s="4"/>
-    </row>
-    <row r="161" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+      <c r="R160" s="4"/>
+    </row>
+    <row r="161" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="9">
         <v>9567976211028970</v>
       </c>
@@ -10189,8 +10393,9 @@
       </c>
       <c r="P161" s="4"/>
       <c r="Q161" s="4"/>
-    </row>
-    <row r="162" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R161" s="4"/>
+    </row>
+    <row r="162" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10238,8 +10443,9 @@
       </c>
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
-    </row>
-    <row r="163" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R162" s="4"/>
+    </row>
+    <row r="163" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10287,8 +10493,9 @@
       </c>
       <c r="P163" s="4"/>
       <c r="Q163" s="4"/>
-    </row>
-    <row r="164" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R163" s="4"/>
+    </row>
+    <row r="164" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10336,8 +10543,9 @@
       </c>
       <c r="P164" s="4"/>
       <c r="Q164" s="4"/>
-    </row>
-    <row r="165" spans="1:17" ht="270" x14ac:dyDescent="0.25">
+      <c r="R164" s="4"/>
+    </row>
+    <row r="165" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10385,8 +10593,9 @@
       </c>
       <c r="P165" s="4"/>
       <c r="Q165" s="4"/>
-    </row>
-    <row r="166" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R165" s="4"/>
+    </row>
+    <row r="166" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10434,8 +10643,9 @@
       </c>
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
-    </row>
-    <row r="167" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R166" s="4"/>
+    </row>
+    <row r="167" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="9">
         <v>9567976211059800</v>
       </c>
@@ -10483,8 +10693,9 @@
       </c>
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
-    </row>
-    <row r="168" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R167" s="4"/>
+    </row>
+    <row r="168" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A168" s="9">
         <v>9567976221086510</v>
       </c>
@@ -10525,19 +10736,22 @@
         <v>468</v>
       </c>
       <c r="N168" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="O168" s="4">
         <v>3</v>
       </c>
       <c r="P168" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="Q168" s="4" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+      <c r="R168" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <v>9567976221086510</v>
       </c>
@@ -10585,8 +10799,9 @@
       </c>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
-    </row>
-    <row r="170" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R169" s="4"/>
+    </row>
+    <row r="170" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <v>9567976221086510</v>
       </c>
@@ -10634,8 +10849,9 @@
       </c>
       <c r="P170" s="4"/>
       <c r="Q170" s="4"/>
-    </row>
-    <row r="171" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R170" s="4"/>
+    </row>
+    <row r="171" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="9">
         <v>9567976221086510</v>
       </c>
@@ -10683,8 +10899,9 @@
       </c>
       <c r="P171" s="4"/>
       <c r="Q171" s="4"/>
-    </row>
-    <row r="172" spans="1:17" ht="300" x14ac:dyDescent="0.25">
+      <c r="R171" s="4"/>
+    </row>
+    <row r="172" spans="1:18" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="9">
         <v>9567976221086510</v>
       </c>
@@ -10732,16 +10949,17 @@
       </c>
       <c r="P172" s="4"/>
       <c r="Q172" s="4"/>
-    </row>
-    <row r="173" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R172" s="4"/>
+    </row>
+    <row r="173" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="9">
         <v>9567976231222830</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D173" s="10"/>
       <c r="E173" s="10"/>
@@ -10759,10 +10977,11 @@
       </c>
       <c r="P173" s="4"/>
       <c r="Q173" s="4" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="174" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+      <c r="R173" s="4"/>
+    </row>
+    <row r="174" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="9">
         <v>9567976231223130</v>
       </c>
@@ -10810,8 +11029,9 @@
       </c>
       <c r="P174" s="4"/>
       <c r="Q174" s="4"/>
-    </row>
-    <row r="175" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R174" s="4"/>
+    </row>
+    <row r="175" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <v>9567976231223130</v>
       </c>
@@ -10859,8 +11079,9 @@
       </c>
       <c r="P175" s="4"/>
       <c r="Q175" s="4"/>
-    </row>
-    <row r="176" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R175" s="4"/>
+    </row>
+    <row r="176" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="9">
         <v>9567976231223130</v>
       </c>
@@ -10908,8 +11129,9 @@
       </c>
       <c r="P176" s="4"/>
       <c r="Q176" s="4"/>
-    </row>
-    <row r="177" spans="1:17" ht="210" x14ac:dyDescent="0.25">
+      <c r="R176" s="4"/>
+    </row>
+    <row r="177" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="9">
         <v>9567976231223130</v>
       </c>
@@ -10957,8 +11179,9 @@
       </c>
       <c r="P177" s="4"/>
       <c r="Q177" s="4"/>
-    </row>
-    <row r="178" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R177" s="4"/>
+    </row>
+    <row r="178" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11006,8 +11229,9 @@
       </c>
       <c r="P178" s="4"/>
       <c r="Q178" s="4"/>
-    </row>
-    <row r="179" spans="1:17" ht="345" x14ac:dyDescent="0.25">
+      <c r="R178" s="4"/>
+    </row>
+    <row r="179" spans="1:18" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11055,8 +11279,9 @@
       </c>
       <c r="P179" s="4"/>
       <c r="Q179" s="4"/>
-    </row>
-    <row r="180" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R179" s="4"/>
+    </row>
+    <row r="180" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11104,8 +11329,9 @@
       </c>
       <c r="P180" s="4"/>
       <c r="Q180" s="4"/>
-    </row>
-    <row r="181" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+      <c r="R180" s="4"/>
+    </row>
+    <row r="181" spans="1:18" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11153,8 +11379,9 @@
       </c>
       <c r="P181" s="4"/>
       <c r="Q181" s="4"/>
-    </row>
-    <row r="182" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R181" s="4"/>
+    </row>
+    <row r="182" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11202,8 +11429,9 @@
       </c>
       <c r="P182" s="4"/>
       <c r="Q182" s="4"/>
-    </row>
-    <row r="183" spans="1:17" ht="270" x14ac:dyDescent="0.25">
+      <c r="R182" s="4"/>
+    </row>
+    <row r="183" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11251,8 +11479,9 @@
       </c>
       <c r="P183" s="4"/>
       <c r="Q183" s="4"/>
-    </row>
-    <row r="184" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+      <c r="R183" s="4"/>
+    </row>
+    <row r="184" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11300,8 +11529,9 @@
       </c>
       <c r="P184" s="4"/>
       <c r="Q184" s="4"/>
-    </row>
-    <row r="185" spans="1:17" ht="270" x14ac:dyDescent="0.25">
+      <c r="R184" s="4"/>
+    </row>
+    <row r="185" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11349,8 +11579,9 @@
       </c>
       <c r="P185" s="4"/>
       <c r="Q185" s="4"/>
-    </row>
-    <row r="186" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+      <c r="R185" s="4"/>
+    </row>
+    <row r="186" spans="1:18" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11398,8 +11629,9 @@
       </c>
       <c r="P186" s="4"/>
       <c r="Q186" s="4"/>
-    </row>
-    <row r="187" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+      <c r="R186" s="4"/>
+    </row>
+    <row r="187" spans="1:18" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="9">
         <v>9567976231223130</v>
       </c>
@@ -11447,8 +11679,9 @@
       </c>
       <c r="P187" s="4"/>
       <c r="Q187" s="4"/>
-    </row>
-    <row r="188" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R187" s="4"/>
+    </row>
+    <row r="188" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="9">
         <v>9567976241239930</v>
       </c>
@@ -11496,8 +11729,9 @@
       </c>
       <c r="P188" s="4"/>
       <c r="Q188" s="4"/>
-    </row>
-    <row r="189" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="R188" s="4"/>
+    </row>
+    <row r="189" spans="1:18" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="9">
         <v>9567976241239930</v>
       </c>
@@ -11518,19 +11752,20 @@
       <c r="L189" s="4"/>
       <c r="M189" s="4"/>
       <c r="N189" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O189" s="4">
         <v>2</v>
       </c>
       <c r="P189" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="Q189" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="190" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="R189" s="4"/>
+    </row>
+    <row r="190" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="9">
         <v>9567976241239930</v>
       </c>
@@ -11578,8 +11813,9 @@
       </c>
       <c r="P190" s="4"/>
       <c r="Q190" s="4"/>
-    </row>
-    <row r="191" spans="1:17" ht="135" x14ac:dyDescent="0.25">
+      <c r="R190" s="4"/>
+    </row>
+    <row r="191" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="9">
         <v>9567976241239930</v>
       </c>
@@ -11627,8 +11863,9 @@
       </c>
       <c r="P191" s="4"/>
       <c r="Q191" s="4"/>
-    </row>
-    <row r="192" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="R191" s="4"/>
+    </row>
+    <row r="192" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="9">
         <v>9567976241279290</v>
       </c>
@@ -11676,8 +11913,9 @@
       </c>
       <c r="P192" s="4"/>
       <c r="Q192" s="4"/>
-    </row>
-    <row r="193" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="R192" s="4"/>
+    </row>
+    <row r="193" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="9">
         <v>9567976241279290</v>
       </c>
@@ -11698,30 +11936,37 @@
       <c r="L193" s="4"/>
       <c r="M193" s="4"/>
       <c r="N193" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O193" s="4">
         <v>2</v>
       </c>
       <c r="P193" s="4" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="Q193" s="4" t="s">
-        <v>631</v>
-      </c>
+        <v>630</v>
+      </c>
+      <c r="R193" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q193" xr:uid="{71956C31-B19E-4264-8709-1F2CE7C8CF56}"/>
+  <autoFilter ref="A1:Q193" xr:uid="{71956C31-B19E-4264-8709-1F2CE7C8CF56}">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514D3154-937E-43F5-A8E6-F89C0CD1E322}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11873,6 +12118,33 @@
         <v>573</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="str">
+        <f>detection_checked!P1</f>
+        <v>disagreement_keyword</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="str">
+        <f>detection_checked!Q1</f>
+        <v>agreement_comment</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="str">
+        <f>detection_checked!R1</f>
+        <v>agree_3_FP_FN</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>